<commit_message>
adding all file from loc to dev branch
</commit_message>
<xml_diff>
--- a/Testdata/TC_101.xlsx
+++ b/Testdata/TC_101.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="My Series" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -28,7 +28,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>8VIAAB+LCAAAAAAAAAPtXFtvG8cV/isLPSVAqdldXkSp4w0oUnKJUJIhUrGVl2C5O5S2Xu6ye5HEN/chCJDaBYomAZK2aR2gaBCgiR/Swk2C9r8Epuw89S/0zMzeuZS4spooyBoGzDmXuZw5c843Z43Br52NTeGEOK5hW7dWpFVxRSCWZuuGdXRrxfdGFamx8pqCt840Yt5RHXVMPBAWQMtyN85c49bKsedNNhA6PT1dPa2u2s4RkkVRQvd2en3tmIzVimG5nmppZCXS0i/XWlFwWx/vEE/VVU/lmrdWuv3uapsYWgdoO6qlHhFnddN3DYu47pblGZ5BXKrpENUj7c7OG3xhirzaWJUwmqPHkpu+YepcLiXJ6YEcDEsGxpgosiiLFbFZkcWBVN2Qaxv15mq9Jr0ZKkaCuKe6Xp84J4bGCH1PHU+YutiURakq1+pNjHKFoK/YAAreM/V9cmK4RG8T03QLWQQFG9jSPFh1MWOKGCV0g46uPoXbjjo5HhieSYqqb9sO0cBQVxp7l5zuOYH9BpMecAfHhuNNO+q0cF8HLnH2JtQaxVQV3LEtr2USxzuYwKYSHfYcGIrn+ASjBcxYqWO4Gvw2LJ/oykg13aRSionv2s59d6JqZBcOLKJ9nFqmrergWZ7heoYWDzrHwHccewI9wuCbtqlvQ6+BcA4j6rlrgYnpsJu2fT+eXR4TMx9g3gB7Ola9UHyOjvvH9umeZU77/tDVHGNI9M5mKJ3Lw/TkBdpt3/XsMcwiJmFOS1Cm8AdOWpaMO0Qzxqp5xwQjukoVekkRcMv37JHhtW3TH1tuOKcMFd+FFQ3IWbTCqI33YHMtanTb6lqhPDdzLiutsG+fRmPOM5gREuSWq4XbPc/ICneAFm7fPIftCF3ltmFCIkjuRYKa9or+MSFerktwDqYxb5umFmVzuuuPh3C8hnDGTtioLkYxH4Ofgq/DvBQR0kWF/R2I4gb7C/OI2HjL0hfLhUwMwyXGUiTgZUgY1mRumqp1H6h3De94txWuJYeDuQUWys/zMJzcialOGTmyUpKGu5Zm+jrhAaFrjZiL0rnxTV3IxnOkHpxxBavWdDCdQAB2jQ0PftxagZS84XoOJP0VRbN9y3OmNHJgFIhepuP6Q4sNoJpL64wc8isfsMZ027e0tq0vP5rOrXNgGd7yM7R9h4fD5VWY9Whk9N0OoTGGBf2l9bUia3KdQuJji4xty9CWtzYYmc5ev8JC3PBULa1B+PlaWt6EvM7THj3rS6s5ABQh0RUapuW6tmYwZw2Oh57QRwuOTIeMVN8EkOZBij2KYm+WjFvu/axMkoQPHDOMgAqFwC5gYE0fr2oAHijOW9XsMSUggJ53+xgl5SkC0siWddRTrSMfMEYUV7L0KP7S/DhwVMuly4kgRSYU5wvhME5xqKPw4LXnM0fgwcsGLkYZOTwg44ntqOYOGMbYDtwuwEsARXZU7zhoQW4ziRYaGcWqkVZ6ZuHELxNjSYovgx74IExmiEyIroWj7VgmpmG6yh04lmZbNY2hw6NqmMrzeLBhMTgM4y9dXEGgGO4B3Lgg+75OphSGx42AzlxWChncgWkgVfr7taZcF+t1QDa0jdmKb9snngAYmABGFCrCQD0Tfi50Ld04MXRfNeEnOB+sjJsnSEGFNJM6eDuM72wKLZhnmpIWAJxxZED6mBeMOLGCckhUx5wmBPkSe7YGcufv/Wf21R/P3/vn7O2/Vp5/+tvZu4//+81Hz55+9uyrrziVr5FL44E6NAmb0WCz2RSrNXCwiISpVRHDxLqveYx2eMigcNTGwdWNNdpb3fbt3iYLJBExVOe5BNFb4dT242afr4INxPYShS7ARZRBGJiCdoqbyE0KvaWdkLR0kr9Ikdvi+dd/e/713xdqBwaLQZa0vt6sSPKlGAxuutKcXITBeqngT4VrFbFekeWEcEYG7/PIH9mpqytVSVwXpTVRioK4HnlxnlCWFfQ0UI9QRo+T2hwXRS6QbIdM5vkD4noRm5+FRCPw0X/85sUX76ekAusGlHQvMDmGX+hgKGywrnf3B0J/72C/vSUMtvrUT2JeQo53foFwMHp0oFJOZVlwyn8mQFaHLCaswFVoRbBHAlG1Y2EKRzFxEFPOlkflA12xy+wsbzu2P+E7klCIqTmSUTjJ1cgJNozH7DkXdWJWjjif6+xfX+YpBAvpxEhW2d/ZFMZW5JeMhlMcTkrwg1P74b+fPX2HBrcnv5s9/XWqh2CcqB4Afg6nKdmM3B5CXpBoMhR8t8+MeV98a00eSeIakSpVaa1Zqa1Xq5VmVYdmQ1RH2ghOl9iE7vtB1vHHd2zD8lxFqrF7VdDC0KtEB2L/4u4Y0iAbk5kS6BkK/oXqbp15wZlXdjFKE3C4azlXoIVzWD49XcUBLvLJnD297pD60sn74qh6SbS73KPQBTvWJxMV4JQdFxciAs/V8fn57k8fn//hy/MPnrx457PZu5/OHn7w/Os/v/j8MY+u5+8/OX/0eZDNswmfzZSWLPiwAiuAaQJdjUDBmfDtg98Llu0JMDPBZ5nn2wcfJjqjE2XoM+4ZMHs0kfQU5kSTylRPSEwlmkNKL1LhCK9NoUo1kgjAij0xtHiQNyu0KxpfGeOV7qDiu0SwAS6/CitJC8fKy+oFKhw63VkTZUkOuHw2dAlD1U2Y/rZpD8HjQgarMGVEUloXK8SybLzbvb3NVi8W4ZPYc3TiUBfkP3B4Z3D5TSRzP4FgpCutdru/tQ9RiOKHZBpstw92DnqtwdYrr9KrXyLRxV9GIgiXBeIJajSJOCi0HLhOQA+GtjchTlj4mpeLVAGTJJSEPC0qMrf+4CTaXIFc9YqBOOBGqVCDMlE12w4PfZKOEsgdJcA4yoPeKIW10UvjarQQDy/mhDO97kpkBuHmCl+OgrPQlVGWB7YoFdvRPHCNSWghJkVzwBPlQ8EF5DmVyP1ziXleFeXlXGI4QAInIZ6W0Ty8QteDnlASiogvhYaWT5AoQUDzCStNQqkMg7LZJElAidCPcgJ9hobSkRoFUQn+7bphsArXkqAAt62amm/SzzJzYvOsKDamXYx9xRi1dHrRyD9WKQnc9h2HRywr+C7e9ycT24k+YSwWYJ8GEzWmXV4PSlad4na3k+ZDO8GlwTvFZtGcNhliDFgcPXZd+i2FSTGbpj4gAiX42s3jJaA+Zvq7/S3HsZ1gQ4LWDnFdcDYU2zIp1HV5yUqPdyEkRG4fJ5aOMRodAnq6F3/UCAl8xnEvtIFRbj5GiYSd8I3gy8f1Oksmw+dJXKM38SXcZGeijGTzCq5V5NIYK12bO15XJXVNWlhJvaxeehOromX987rqn3Vxycu6/D3VP5vL1D+bZf2zrH+W9c9cBC8trn9Kb43qI70urQ8rWp2MKjVZGlbU5rpWUWuNalMlVUlVc+ufjeoPX//MzOHG1j+vI6QumYwvjp1llbOscv6oqpzSD1vlXJPKKmdZ5SyrnGWVs6xyllXOsspZVjl/OlXO5a+GN7nK2UhVOd9QTZ8IsMVEFwyL/pcR34WUmFfwXCh6M2qfLx4/fPb0o9knH8/e/cvswTdl+fO6yp/N2nJ3dbHx/ZQ/5cYS5U8uVJY/y/LnTSp/9l7fX1D+DDkXlj/PP/jiu3cezt5+Mnv0ePbok/Mv3nvJOqi8uA4qv6UPR6I6lEeVkSiRSq06XK8015pihTRGVVETpfU1qZpXB5VvQB1UvlF10PTmXndsLZ6jL46nZUm0LIn+qEqi8g9cEm2UJdGyJFqWRMuSaFkSLUuiZUm0LIn+dEqiy98S/y8l0eAHf74h9NEOMQGsFX3wKdTesU+urAtuUVS16+6ZemDnYu8HRGaJO0g+v0V9qOhkWo4D4IG+11P4vayeYd3vFlu90pTEui7L8E+DVBtDtao29bVqtVGXxTVtBF7DO6VYnnYxBohHH2MoNohEQ09SPX44Y1+1jgr2xg3MFOnjEmApdlaD+1zUxtuG43r3aH4PfnHKYUQ55JjwHn11iv9g7UOlJnECCKDkYCg16zD0ePylNtvsGWOj4AMUYhif0p2AG0wmHOIV3VC46u6SMw+jRA8AB4a/BOTBX2wp0hs/VXC3ifTDvvr+sHB3KFS+A3zqWFfT3tIBOV5dm717ZpgvMQGGF6/aRddyjaNjr+i+yuvrVdIgckUeaRr9z/2kAnhvWNHV0bokiqOqXpfpE1VB55A4DHJacBCabgzXV83ieijzcKXyP3F72QnxUgAA</t>
+          <t>p1EAAB+LCAAAAAAAAAPtXFtv48YV/iuEnxIg9JCSLMvuLANZsrdCZHthydl1iiKgyJHNLkWqvNjWW/oQBEiTAkWTAEnbtBugaBCgyT6kxTYJ2v8SrL2bp/6FnpnhZUhRtuR1sg7CxWJXcy4zZ2bOnPPNIUH88unIlo6J51uuc2tJXVaWJOIYrmk5h7eWwmAoq/WllzW8eWoQ+47u6SMSgLAEWo6/fupbt5aOgmC8jtDJycnySXXZ9Q5RRVFUdG+72zOOyEiXLccPdMcgS4mWebnWkoZb5mibBLqpBzrXvLXU6XWWW8Qy2kDb1h39kHjLG6FvOcT3N53ACiziU02P6AFptbdf5RPTKsv1ZRWjKXoquRFatsnlMpKcHsnBsKRvjYhWUdSGrKzJSrWv1NerlXWltry2tvJarJgI4q7uBz3iHVsGI/QCfTRm6sqaUlXq1YpSw6hQCPpKF0DDu7a5R44tn5gtYtv+QiuCog1sGgHMerHFVDASdKOOrm7CbU8fH/WtwCaLmbG3vSGNnJek7it78H9kU9qZhrdcjxiwjlcybYec7HrR8vbHXeD2jywvmLT1ycJ97fvE2x3TxVpMVcNt1wmaNvGC/THsOTHBJYChBV5IMJrBTJXalm/Ab8sJiakNddsXlTJMfNf17vtj3SA7cJ4R7ePEsV3dBMcLLD+wjHTQKQa+47lj6BEG33Btcwt6jYQLGEnPHQeWmA674br3U+uKmJjtKttf2NORHsTiU3TcO3JPdh170gsHvuFZA2K2N2LpQh6mBzPSboV+4I7AipSEOU2gTOAPHMQ8GbeJYY10+44Ni+hrVeglQ8DNMHCHVtBy7XDk+LFNOSq+CzPqk9Nkhkkb78LmOnTRXafjxPJ8mQtZWYU99yQZc5rBFkEgN30j3u5pRl64DbR4+6Y5bEfoLLcsG/KEuBcCNesVvSNCgkKX4BxMQ+IWzTzaxmQnHA3geA3gjB2zUX2MUj4GPwVfB7s0BbKJzP72FWWd/QU7EjbedMzZcjETw3DCWJoKvBwJw5zsDVt37gP1rhUc7TTjuRRwMF+BmfLTPAwnd2zrE0ZOVkmk4Y5j2KFJeEDoOEPmotQ2vqkz2XiK1IUzrmHdmfQnY4jPvrUewI9bS5Cx1/3AA0ywpBlu6ATehEYOjCLRy3T8cOCwAXR7bp2hR34dAhSZbIWO0XLN+Ucz+ersO1Ywv4Vu6PFwOL8KWz0aGUO/TWiMYUF/bn1jkTn53kLiI4eMXMcy5l9tWGRqvXmFifjxqZpbg/DzNbe8DXmdpz161udW8wBHQqJbaJim77uGxZw1Oh6moI9mHJk2GeqhDRgugBR7mMTePBk3/ft5GZGE9z07joAaRcg+QGTDHC0bAB4oDFw23BElIECmd3sYifIUARlk0zns6s5hCBgjiSt5ehJ/aX7se7rj0+kkkCIXiouFcBynONTRePDaDZkj8ODlAhejnBzuk9HY9XR7GxbG2orcLsJLAEW29eAoakFus4kRLzJKVROtrGWx4ZeJsSTFp0EPfBQmc0QmROfCwXgqk9IwneU2HEu7pdvWwONRNU7lRTzYsBQcxvGXTm5BoBjvAVzIIPu+QiYUpaeNiM5cVo0Z3IFpINV6e7VGZUVZWQFkQ9uYzfi2exxIgIEJYERJlvr6qfQzqeOY1rFlhroNP8H5iPSLZqu1v73fbfY3X3jxl5AP2WpFGelZOhK7wFtx9GcGNmEWWUpWAFDIoQXJZVow4aQK2gHRPXsiCPIF6LoGyJ2/99+zr/50/t6/zt78m/zk09+dvf3gf9989PjRZ4+/+opTC1eAK+O+PrAJM7C/0WgoVbjbpSRMtwAxAG2GRsBoBwcMNydtHF0DWaO12Wnd7m6wqJMQY3WeeBC9YU7cMG32+KTYQGzjUewvXETrx1Esame4QiLT6I3vmGSlRf4sRb4WT77++5Ov/zFTO1qwFJGpa2sNWa1cCtjg7qxOySWArZvJFFS4JisrcqUiCOdk8B5PE8k6dUytqsL1XF1V1CTim4mPFwnlWVFPff0Q5fQ4qcVBVOICYjtmsoPQJ36QsPnREBqRy/7zt0+/eD8jFa1uRMn2AsYxsEMHQ3GDdb2z15d6u/t7rU2pv9mjfpLyBDne+QXC0ejJ+co4leNADHhJAggAKU9agnvTkuQOJaIbR9IETqZwLjPOVkTlA12xy7yVtz03HPMdERRSaoFkEl0KNQpiD+Ox9ZwKQimrQJzbevbvL4sUoom0U9gbVUsSv2Q0nOFwksCPTu2H/3n86C0a6x7+/uzRbzI9ROMkxQPwczhNYjNxewh5UVbKUfDdHlvM+8rrg+GqaawNa3Kj3jDkmlnX5cGgtiqvKWsNc3XFrA3rkKAieXoTu+NaTuBrao1dwqIWhl5VOhD7H3dGkDPZmGwpgZ6j4J/r/uZpEJ15bQejLAHHu1ZwX5ppw/zZ6ioOcJFPFuzpdYfUxVN7LpdfHFUviXaXexS6YMd6ZKwD9nLTSkRC4Lk6PT/f/fnj8z9+ef7Bw6dvfXb29qdn73zw5Ou/PP38AY+u5+8/PH/38yib5xM+s5TWN/iwEquWGRKdjUSRnPTtG3+QHDeQwDIpZJnn2zc+FDqjhjKomvYMAD8xJGvClKioTPUkwZTEhoxeosLhYItClWoiEYEVd2wZ6SCvybQrGl8Z44VOXw59IrmArV+EmWSFU+V59SIVDp3urCoVtRJxuTV0CgPdF5b+tu0OwONiBitH5UQyWhcrpLJsvNvd3Y1mNxXhRux6JvGoC/IfOL5g+PzakrvMQDAyNYCKvc09iEIUP4hpUICQ9J4oJLr0KUsC4fKoXaAmRqRBoenB3QN6sIzdMfHiKtm0XKIKmERQkoq0qMjU/KOT6HIFctX7COL4G2VCDcpF1Xw7PvQiHQlAHglgHBVBb5TB2uiZcTWaiYdnc2JLr7tsmUO4hcKXo+A8dGWU+YEtysR2NA1cUxKaiUnRFPBExVBwBnlKJXH/QmKRVyV5uZAYDyDgJMTTMpqGV+h60BMSoYjyTGho/gSJBAKaTlhZEspkGJTPJiIBCaEfFQT6HA1lIzWKohISojH87vhxK56XQAFuS7eN0KbPc6bEpllJz1l3Y48/hk2TXjqKj1hGArdCz+PRy4met/fC8dj1kmcfswXYM0WhOLXDC0liuSptd9pZPrQFLg3kGTaL7LTJ0GPE4kiy49OHMEyKrWnmySNQoqfoPHYCAmTbcLe36XmuF21O1Nomvg+OJ+ySKNTxea3LTHchJiRHIE0ybWs4PAAkdS99GhITuMVpL7SBUWFuRkLyFnwjemRyvc6Sy/ZFEtfoTXwKN9mZKENsXsG1FrlApkrX5o7XVYJdrWdKsK/qNtyrYIuJKVkOvViFPqTHOWqu82rejCLr0wfvPH700dknH5+9/dezN74pK6rfU0W1UZvv+q/Uf5iKaqU+R0WVC5UV1bKiepMqqvF7Z9MV1ZhzYUX1/IMvvnvrnbM3H569++Ds3U/Ov3jvGUur6uzSqvp6w1RXDbU6lHViDuWaUVVlvWYastIA8mBYWV1prBWVVivV519azdnwnEur2c297tg6Rwa/sJaaj6dlLbWspf6oaqnq862lUvhd1lLLWmpZSy1rqWUttayllrXUspb6U6ylzn9jvMm1VHX266wLvrR6M6um4qupZcn0eyqZrihzvjFV+YFeQm3M8xJqoyyZliXTm1YyvSEvoVZmV0orr1eH5sBQhqsy0QemXCOKIuvKiiqT4crqoL4G2KFKiiql9RtQKa3fqErp7JdQryOkzkrVF79q2ijLo2V59EdcHq085/KoWpZHy/JoWR4ty6NlebQsj5bl0bI8+tMsj85/TfxeyqPRD/6lidhH28QG4Lbot6li7W33+Mq64BaLqnb8XduM1nmxTx0ky5J2IH5IjPrQdX1HjPtj0/MAZtAPDy384a/4gxl7unO4oFV8SkyRfnkCRo9RgOX5wT2aTqNfnHKQUA44BLtHv0HFf7D2gVZTOQEEkNg7ypgZn+6Af9bNtbvWyFrwcxRKHAKyncBajsccUXUW8xh6s9whp3A/F3qA7Dv4FSR6/v2WRXrjjgtXiUSffjPJtw6PgkUNWx3oxCQDRTYGpCLXTKUhrxFSlVUV/tWNSkVRVugXl6LOIbhY5GTBQVC8YentTPs/1twoIKdRAAA=</t>
         </r>
       </text>
     </comment>
@@ -42,7 +42,7 @@
     <numFmt numFmtId="164" formatCode="yyyy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="164" formatCode="yyyy"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="###0.000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -418,17 +418,17 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>Govt Revenue - Tax ; Individual Income</t>
+          <t>Govt Revenue - Tax ; Individual Income [ACCUMULATE()]</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>Govt Revenue</t>
+          <t>Value Added in Industry [ACCUMULATE()]</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>Value Added in Industry</t>
+          <t>Govt Revenue [ACCUMULATE()]</t>
         </is>
       </c>
     </row>
@@ -499,12 +499,12 @@
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
+          <t>LKR mn</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
           <t>RMB mn</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>LKR mn</t>
         </is>
       </c>
     </row>
@@ -562,10 +562,10 @@
         <v>310901701</v>
       </c>
       <c r="C8" s="3">
+        <v>310902601</v>
+      </c>
+      <c r="D8" s="3">
         <v>310901801</v>
-      </c>
-      <c r="D8" s="3">
-        <v>310902601</v>
       </c>
     </row>
     <row r="9">
@@ -581,12 +581,12 @@
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
+          <t>SR4825076</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
           <t>SR4825071</t>
-        </is>
-      </c>
-      <c r="D9" s="2" t="inlineStr">
-        <is>
-          <t>SR4825076</t>
         </is>
       </c>
     </row>
@@ -603,7 +603,7 @@
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>Function Description</t>
+          <t>Function Information</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
@@ -632,10 +632,10 @@
         <v>36130</v>
       </c>
       <c r="C12" s="4">
+        <v>31017</v>
+      </c>
+      <c r="D12" s="4">
         <v>18598</v>
-      </c>
-      <c r="D12" s="4">
-        <v>31017</v>
       </c>
     </row>
     <row r="13">
@@ -648,10 +648,10 @@
         <v>40878</v>
       </c>
       <c r="C13" s="4">
+        <v>39052</v>
+      </c>
+      <c r="D13" s="4">
         <v>41244</v>
-      </c>
-      <c r="D13" s="4">
-        <v>39052</v>
       </c>
     </row>
     <row r="14">
@@ -700,10 +700,10 @@
         <v>8280.155000000001</v>
       </c>
       <c r="C17" s="2">
+        <v>1453915.3</v>
+      </c>
+      <c r="D17" s="2">
         <v>37803803.9</v>
-      </c>
-      <c r="D17" s="2">
-        <v>1453915.3</v>
       </c>
     </row>
     <row r="18">
@@ -716,10 +716,10 @@
         <v>18439868.19811667</v>
       </c>
       <c r="C18" s="2">
+        <v>407944167687.1222</v>
+      </c>
+      <c r="D18" s="2">
         <v>310352334867253.9</v>
-      </c>
-      <c r="D18" s="2">
-        <v>407944167687.1222</v>
       </c>
     </row>
     <row r="19">
@@ -732,10 +732,10 @@
         <v>4294.166764125104</v>
       </c>
       <c r="C19" s="2">
+        <v>638705.0709733892</v>
+      </c>
+      <c r="D19" s="2">
         <v>17616819.65813506</v>
-      </c>
-      <c r="D19" s="2">
-        <v>638705.0709733892</v>
       </c>
     </row>
     <row r="20">
@@ -748,10 +748,10 @@
         <v>0.396554507119883</v>
       </c>
       <c r="C20" s="2">
-        <v>0.4216272309807009</v>
+        <v>0.4485025925517874</v>
       </c>
       <c r="D20" s="2">
-        <v>0.4485025925517873</v>
+        <v>0.421627230980701</v>
       </c>
     </row>
     <row r="21">
@@ -761,13 +761,13 @@
         </is>
       </c>
       <c r="B21" s="2">
-        <v>-1.129868563809902</v>
+        <v>-1.129868563809901</v>
       </c>
       <c r="C21" s="2">
+        <v>-0.9169323140962309</v>
+      </c>
+      <c r="D21" s="2">
         <v>-1.334739153466928</v>
-      </c>
-      <c r="D21" s="2">
-        <v>-0.9169323140962304</v>
       </c>
     </row>
     <row r="22">
@@ -780,10 +780,10 @@
         <v>0.5186094661422527</v>
       </c>
       <c r="C22" s="2">
+        <v>0.4393000548060738</v>
+      </c>
+      <c r="D22" s="2">
         <v>0.4660065348115686</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0.4393000548060738</v>
       </c>
     </row>
     <row r="23">
@@ -796,10 +796,10 @@
         <v>2912.2</v>
       </c>
       <c r="C23" s="2">
+        <v>643058</v>
+      </c>
+      <c r="D23" s="2">
         <v>16641896</v>
-      </c>
-      <c r="D23" s="2">
-        <v>643058</v>
       </c>
     </row>
     <row r="24">
@@ -812,10 +812,10 @@
         <v>15339.82</v>
       </c>
       <c r="C24" s="2">
+        <v>2549974</v>
+      </c>
+      <c r="D24" s="2">
         <v>63990353</v>
-      </c>
-      <c r="D24" s="2">
-        <v>2549974</v>
       </c>
     </row>
     <row r="25">
@@ -828,10 +828,10 @@
         <v>7666.385</v>
       </c>
       <c r="C25" s="2">
+        <v>1362529.5</v>
+      </c>
+      <c r="D25" s="2">
         <v>34521187.5</v>
-      </c>
-      <c r="D25" s="2">
-        <v>1362529.5</v>
       </c>
     </row>
     <row r="26">
@@ -855,50 +855,50 @@
         <v>35765</v>
       </c>
       <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8">
+      <c r="C27" s="8">
         <v>643058</v>
       </c>
+      <c r="D27" s="8"/>
     </row>
     <row r="28">
       <c r="A28" s="7">
         <v>36130</v>
       </c>
       <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8">
+      <c r="C28" s="8">
         <v>772535</v>
       </c>
+      <c r="D28" s="8"/>
     </row>
     <row r="29">
       <c r="A29" s="7">
         <v>36495</v>
       </c>
       <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8">
+      <c r="C29" s="8">
         <v>915947</v>
       </c>
+      <c r="D29" s="8"/>
     </row>
     <row r="30">
       <c r="A30" s="7">
         <v>36861</v>
       </c>
       <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8">
+      <c r="C30" s="8">
         <v>1083440</v>
       </c>
+      <c r="D30" s="8"/>
     </row>
     <row r="31">
       <c r="A31" s="7">
         <v>37226</v>
       </c>
       <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8">
+      <c r="C31" s="8">
         <v>1262998</v>
       </c>
+      <c r="D31" s="8"/>
     </row>
     <row r="32">
       <c r="A32" s="7">
@@ -907,10 +907,10 @@
       <c r="B32" s="8">
         <v>2912.2</v>
       </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8">
+      <c r="C32" s="8">
         <v>1462061</v>
       </c>
+      <c r="D32" s="8"/>
     </row>
     <row r="33">
       <c r="A33" s="7">
@@ -920,10 +920,10 @@
         <v>3639.83</v>
       </c>
       <c r="C33" s="8">
+        <v>1683077</v>
+      </c>
+      <c r="D33" s="8">
         <v>16641896</v>
-      </c>
-      <c r="D33" s="8">
-        <v>1683077</v>
       </c>
     </row>
     <row r="34">
@@ -934,10 +934,10 @@
         <v>4562.74</v>
       </c>
       <c r="C34" s="8">
+        <v>1939649</v>
+      </c>
+      <c r="D34" s="8">
         <v>19281543</v>
-      </c>
-      <c r="D34" s="8">
-        <v>1939649</v>
       </c>
     </row>
     <row r="35">
@@ -948,10 +948,10 @@
         <v>5689.23</v>
       </c>
       <c r="C35" s="8">
+        <v>2226414</v>
+      </c>
+      <c r="D35" s="8">
         <v>22446472</v>
-      </c>
-      <c r="D35" s="8">
-        <v>2226414</v>
       </c>
     </row>
     <row r="36">
@@ -962,10 +962,10 @@
         <v>6925.03</v>
       </c>
       <c r="C36" s="8">
+        <v>2549974</v>
+      </c>
+      <c r="D36" s="8">
         <v>26322492</v>
-      </c>
-      <c r="D36" s="8">
-        <v>2549974</v>
       </c>
     </row>
     <row r="37">
@@ -975,10 +975,10 @@
       <c r="B37" s="8">
         <v>8407.74</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C37" s="8"/>
+      <c r="D37" s="8">
         <v>31454670</v>
       </c>
-      <c r="D37" s="8"/>
     </row>
     <row r="38">
       <c r="A38" s="7">
@@ -987,10 +987,10 @@
       <c r="B38" s="8">
         <v>10006.35</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C38" s="8"/>
+      <c r="D38" s="8">
         <v>37587705</v>
       </c>
-      <c r="D38" s="8"/>
     </row>
     <row r="39">
       <c r="A39" s="7">
@@ -999,10 +999,10 @@
       <c r="B39" s="8">
         <v>11645.89</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C39" s="8"/>
+      <c r="D39" s="8">
         <v>44439535</v>
       </c>
-      <c r="D39" s="8"/>
     </row>
     <row r="40">
       <c r="A40" s="7">
@@ -1011,10 +1011,10 @@
       <c r="B40" s="8">
         <v>13672.72</v>
       </c>
-      <c r="C40" s="8">
+      <c r="C40" s="8"/>
+      <c r="D40" s="8">
         <v>52749686</v>
       </c>
-      <c r="D40" s="8"/>
     </row>
     <row r="41">
       <c r="A41" s="7">
@@ -1023,78 +1023,23 @@
       <c r="B41" s="8">
         <v>15339.82</v>
       </c>
-      <c r="C41" s="8">
+      <c r="C41" s="8"/>
+      <c r="D41" s="8">
         <v>63123687</v>
       </c>
-      <c r="D41" s="8"/>
     </row>
     <row r="42">
       <c r="A42" s="7">
         <v>41244</v>
       </c>
       <c r="B42" s="8"/>
-      <c r="C42" s="8">
+      <c r="C42" s="8"/>
+      <c r="D42" s="8">
         <v>63990353</v>
       </c>
-      <c r="D42" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<MetadataExcelFile xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:xsd="http://www.w3.org/2001/XMLSchema">
-  <MetadataLink>
-    <MetadataLink>
-      <SheetId>My Series</SheetId>
-      <LinkPosRow>1</LinkPosRow>
-      <LinkPosCol>1</LinkPosCol>
-      <MetaDataSeries>
-        <MetadataSeries>
-          <InitRow>1</InitRow>
-          <InitCol>2</InitCol>
-          <EndRow>42</EndRow>
-          <EndCol>2</EndCol>
-          <Name>Govt Revenue - Tax ; Individual Income</Name>
-          <DisplayName>Govt Revenue - Tax ; Individual Income</DisplayName>
-          <SeriesId>310901701</SeriesId>
-          <Code>SR4825055</Code>
-          <Order>0</Order>
-        </MetadataSeries>
-        <MetadataSeries>
-          <InitRow>1</InitRow>
-          <InitCol>3</InitCol>
-          <EndRow>42</EndRow>
-          <EndCol>3</EndCol>
-          <Name>Govt Revenue</Name>
-          <DisplayName>Govt Revenue</DisplayName>
-          <SeriesId>310901801</SeriesId>
-          <Code>SR4825071</Code>
-          <Order>1</Order>
-        </MetadataSeries>
-        <MetadataSeries>
-          <InitRow>1</InitRow>
-          <InitCol>4</InitCol>
-          <EndRow>42</EndRow>
-          <EndCol>4</EndCol>
-          <Name>Value Added in Industry</Name>
-          <DisplayName>Value Added in Industry</DisplayName>
-          <SeriesId>310902601</SeriesId>
-          <Code>SR4825076</Code>
-          <Order>2</Order>
-        </MetadataSeries>
-      </MetaDataSeries>
-    </MetadataLink>
-  </MetadataLink>
-</MetadataExcelFile>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61D2AC56-670D-4540-8EE4-6D854BA6CF96}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>